<commit_message>
[Fonds de solidarite] Correct data and fix bug
</commit_message>
<xml_diff>
--- a/published-data/2020-05-05/fonds-solidarite-volet-1-regional-naf.xlsx
+++ b/published-data/2020-05-05/fonds-solidarite-volet-1-regional-naf.xlsx
@@ -663,10 +663,10 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>3608</v>
+        <v>3594</v>
       </c>
       <c r="D2">
-        <v>4894581</v>
+        <v>4876808</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -715,10 +715,10 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>8601</v>
+        <v>8581</v>
       </c>
       <c r="D4">
-        <v>10893849</v>
+        <v>10877247</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -767,10 +767,10 @@
         <v>9</v>
       </c>
       <c r="C6">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="D6">
-        <v>517832</v>
+        <v>513669</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -793,10 +793,10 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <v>24202</v>
+        <v>24160</v>
       </c>
       <c r="D7">
-        <v>34918013</v>
+        <v>34864839</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -819,10 +819,10 @@
         <v>9</v>
       </c>
       <c r="C8">
-        <v>32438</v>
+        <v>32409</v>
       </c>
       <c r="D8">
-        <v>43596046</v>
+        <v>43568235</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -845,10 +845,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>6528</v>
+        <v>6514</v>
       </c>
       <c r="D9">
-        <v>9050006</v>
+        <v>9035914</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -871,10 +871,10 @@
         <v>9</v>
       </c>
       <c r="C10">
-        <v>25011</v>
+        <v>24982</v>
       </c>
       <c r="D10">
-        <v>36049192</v>
+        <v>36019009</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
@@ -897,10 +897,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>3274</v>
+        <v>3258</v>
       </c>
       <c r="D11">
-        <v>4287514</v>
+        <v>4270216</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
@@ -923,10 +923,10 @@
         <v>9</v>
       </c>
       <c r="C12">
-        <v>1471</v>
+        <v>1469</v>
       </c>
       <c r="D12">
-        <v>2077566</v>
+        <v>2074566</v>
       </c>
       <c r="E12" t="s">
         <v>10</v>
@@ -949,10 +949,10 @@
         <v>9</v>
       </c>
       <c r="C13">
-        <v>5606</v>
+        <v>5592</v>
       </c>
       <c r="D13">
-        <v>7710379</v>
+        <v>7690493</v>
       </c>
       <c r="E13" t="s">
         <v>10</v>
@@ -975,10 +975,10 @@
         <v>9</v>
       </c>
       <c r="C14">
-        <v>17448</v>
+        <v>17391</v>
       </c>
       <c r="D14">
-        <v>23629524</v>
+        <v>23560096</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
@@ -1001,10 +1001,10 @@
         <v>9</v>
       </c>
       <c r="C15">
-        <v>8443</v>
+        <v>8423</v>
       </c>
       <c r="D15">
-        <v>10923966</v>
+        <v>10899879</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1053,10 +1053,10 @@
         <v>9</v>
       </c>
       <c r="C17">
-        <v>18972</v>
+        <v>18905</v>
       </c>
       <c r="D17">
-        <v>24384971</v>
+        <v>24313191</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
@@ -1079,10 +1079,10 @@
         <v>9</v>
       </c>
       <c r="C18">
-        <v>22063</v>
+        <v>21987</v>
       </c>
       <c r="D18">
-        <v>29795751</v>
+        <v>29718715</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
@@ -1105,10 +1105,10 @@
         <v>9</v>
       </c>
       <c r="C19">
-        <v>9165</v>
+        <v>9140</v>
       </c>
       <c r="D19">
-        <v>11221803</v>
+        <v>11199363</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
@@ -1131,10 +1131,10 @@
         <v>9</v>
       </c>
       <c r="C20">
-        <v>27502</v>
+        <v>27429</v>
       </c>
       <c r="D20">
-        <v>33993707</v>
+        <v>33936868</v>
       </c>
       <c r="E20" t="s">
         <v>10</v>
@@ -1157,10 +1157,10 @@
         <v>9</v>
       </c>
       <c r="C21">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="D21">
-        <v>1796600</v>
+        <v>1793720</v>
       </c>
       <c r="E21" t="s">
         <v>11</v>
@@ -1209,10 +1209,10 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>2446</v>
+        <v>2442</v>
       </c>
       <c r="D23">
-        <v>3037794</v>
+        <v>3035808</v>
       </c>
       <c r="E23" t="s">
         <v>11</v>
@@ -1287,10 +1287,10 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>5970</v>
+        <v>5962</v>
       </c>
       <c r="D26">
-        <v>8578900</v>
+        <v>8569380</v>
       </c>
       <c r="E26" t="s">
         <v>11</v>
@@ -1313,10 +1313,10 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>10353</v>
+        <v>10349</v>
       </c>
       <c r="D27">
-        <v>13810027</v>
+        <v>13805961</v>
       </c>
       <c r="E27" t="s">
         <v>11</v>
@@ -1365,10 +1365,10 @@
         <v>9</v>
       </c>
       <c r="C29">
-        <v>7358</v>
+        <v>7354</v>
       </c>
       <c r="D29">
-        <v>10511896</v>
+        <v>10505896</v>
       </c>
       <c r="E29" t="s">
         <v>11</v>
@@ -1391,10 +1391,10 @@
         <v>9</v>
       </c>
       <c r="C30">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="D30">
-        <v>793971</v>
+        <v>784971</v>
       </c>
       <c r="E30" t="s">
         <v>11</v>
@@ -1443,10 +1443,10 @@
         <v>9</v>
       </c>
       <c r="C32">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="D32">
-        <v>1732178</v>
+        <v>1728536</v>
       </c>
       <c r="E32" t="s">
         <v>11</v>
@@ -1469,10 +1469,10 @@
         <v>9</v>
       </c>
       <c r="C33">
-        <v>3442</v>
+        <v>3436</v>
       </c>
       <c r="D33">
-        <v>4642715</v>
+        <v>4635515</v>
       </c>
       <c r="E33" t="s">
         <v>11</v>
@@ -1495,10 +1495,10 @@
         <v>9</v>
       </c>
       <c r="C34">
-        <v>1836</v>
+        <v>1834</v>
       </c>
       <c r="D34">
-        <v>2316867</v>
+        <v>2313867</v>
       </c>
       <c r="E34" t="s">
         <v>11</v>
@@ -1547,10 +1547,10 @@
         <v>9</v>
       </c>
       <c r="C36">
-        <v>2676</v>
+        <v>2670</v>
       </c>
       <c r="D36">
-        <v>3232552</v>
+        <v>3229691</v>
       </c>
       <c r="E36" t="s">
         <v>11</v>
@@ -1573,10 +1573,10 @@
         <v>9</v>
       </c>
       <c r="C37">
-        <v>4805</v>
+        <v>4799</v>
       </c>
       <c r="D37">
-        <v>6460927</v>
+        <v>6454865</v>
       </c>
       <c r="E37" t="s">
         <v>11</v>
@@ -1599,10 +1599,10 @@
         <v>9</v>
       </c>
       <c r="C38">
-        <v>2259</v>
+        <v>2255</v>
       </c>
       <c r="D38">
-        <v>2709643</v>
+        <v>2708719</v>
       </c>
       <c r="E38" t="s">
         <v>11</v>
@@ -1625,10 +1625,10 @@
         <v>9</v>
       </c>
       <c r="C39">
-        <v>8617</v>
+        <v>8599</v>
       </c>
       <c r="D39">
-        <v>10780205</v>
+        <v>10771746</v>
       </c>
       <c r="E39" t="s">
         <v>11</v>
@@ -1651,10 +1651,10 @@
         <v>9</v>
       </c>
       <c r="C40">
-        <v>1224</v>
+        <v>1222</v>
       </c>
       <c r="D40">
-        <v>1672124</v>
+        <v>1669124</v>
       </c>
       <c r="E40" t="s">
         <v>12</v>
@@ -1703,10 +1703,10 @@
         <v>9</v>
       </c>
       <c r="C42">
-        <v>3279</v>
+        <v>3275</v>
       </c>
       <c r="D42">
-        <v>3950416</v>
+        <v>3947402</v>
       </c>
       <c r="E42" t="s">
         <v>12</v>
@@ -1781,10 +1781,10 @@
         <v>9</v>
       </c>
       <c r="C45">
-        <v>6771</v>
+        <v>6769</v>
       </c>
       <c r="D45">
-        <v>9706663</v>
+        <v>9703663</v>
       </c>
       <c r="E45" t="s">
         <v>12</v>
@@ -1807,10 +1807,10 @@
         <v>9</v>
       </c>
       <c r="C46">
-        <v>11440</v>
+        <v>11433</v>
       </c>
       <c r="D46">
-        <v>15462578</v>
+        <v>15453757</v>
       </c>
       <c r="E46" t="s">
         <v>12</v>
@@ -1833,10 +1833,10 @@
         <v>9</v>
       </c>
       <c r="C47">
-        <v>1213</v>
+        <v>1211</v>
       </c>
       <c r="D47">
-        <v>1639200</v>
+        <v>1638666</v>
       </c>
       <c r="E47" t="s">
         <v>12</v>
@@ -1859,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="C48">
-        <v>9935</v>
+        <v>9933</v>
       </c>
       <c r="D48">
-        <v>14281573</v>
+        <v>14280828</v>
       </c>
       <c r="E48" t="s">
         <v>12</v>
@@ -1885,10 +1885,10 @@
         <v>9</v>
       </c>
       <c r="C49">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="D49">
-        <v>1248216</v>
+        <v>1246706</v>
       </c>
       <c r="E49" t="s">
         <v>12</v>
@@ -1937,10 +1937,10 @@
         <v>9</v>
       </c>
       <c r="C51">
-        <v>1841</v>
+        <v>1833</v>
       </c>
       <c r="D51">
-        <v>2432803</v>
+        <v>2425872</v>
       </c>
       <c r="E51" t="s">
         <v>12</v>
@@ -1963,10 +1963,10 @@
         <v>9</v>
       </c>
       <c r="C52">
-        <v>5158</v>
+        <v>5148</v>
       </c>
       <c r="D52">
-        <v>6947209</v>
+        <v>6936130</v>
       </c>
       <c r="E52" t="s">
         <v>12</v>
@@ -1989,10 +1989,10 @@
         <v>9</v>
       </c>
       <c r="C53">
-        <v>2270</v>
+        <v>2266</v>
       </c>
       <c r="D53">
-        <v>2827236</v>
+        <v>2826238</v>
       </c>
       <c r="E53" t="s">
         <v>12</v>
@@ -2015,10 +2015,10 @@
         <v>9</v>
       </c>
       <c r="C54">
-        <v>2892</v>
+        <v>2888</v>
       </c>
       <c r="D54">
-        <v>3549956</v>
+        <v>3546882</v>
       </c>
       <c r="E54" t="s">
         <v>12</v>
@@ -2041,10 +2041,10 @@
         <v>9</v>
       </c>
       <c r="C55">
-        <v>7958</v>
+        <v>7946</v>
       </c>
       <c r="D55">
-        <v>10837794</v>
+        <v>10823092</v>
       </c>
       <c r="E55" t="s">
         <v>12</v>
@@ -2067,10 +2067,10 @@
         <v>9</v>
       </c>
       <c r="C56">
-        <v>2713</v>
+        <v>2711</v>
       </c>
       <c r="D56">
-        <v>3239596</v>
+        <v>3237375</v>
       </c>
       <c r="E56" t="s">
         <v>12</v>
@@ -2093,10 +2093,10 @@
         <v>9</v>
       </c>
       <c r="C57">
-        <v>9722</v>
+        <v>9710</v>
       </c>
       <c r="D57">
-        <v>12221385</v>
+        <v>12216552</v>
       </c>
       <c r="E57" t="s">
         <v>12</v>
@@ -2145,10 +2145,10 @@
         <v>9</v>
       </c>
       <c r="C59">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="D59">
-        <v>2552033</v>
+        <v>2549033</v>
       </c>
       <c r="E59" t="s">
         <v>13</v>
@@ -2223,10 +2223,10 @@
         <v>9</v>
       </c>
       <c r="C62">
-        <v>5999</v>
+        <v>5997</v>
       </c>
       <c r="D62">
-        <v>8583929</v>
+        <v>8580929</v>
       </c>
       <c r="E62" t="s">
         <v>13</v>
@@ -2249,10 +2249,10 @@
         <v>9</v>
       </c>
       <c r="C63">
-        <v>8480</v>
+        <v>8476</v>
       </c>
       <c r="D63">
-        <v>11175780</v>
+        <v>11173225</v>
       </c>
       <c r="E63" t="s">
         <v>13</v>
@@ -2379,10 +2379,10 @@
         <v>9</v>
       </c>
       <c r="C68">
-        <v>1357</v>
+        <v>1355</v>
       </c>
       <c r="D68">
-        <v>1836287</v>
+        <v>1833287</v>
       </c>
       <c r="E68" t="s">
         <v>13</v>
@@ -2405,10 +2405,10 @@
         <v>9</v>
       </c>
       <c r="C69">
-        <v>3315</v>
+        <v>3313</v>
       </c>
       <c r="D69">
-        <v>4477008</v>
+        <v>4474008</v>
       </c>
       <c r="E69" t="s">
         <v>13</v>
@@ -2431,10 +2431,10 @@
         <v>9</v>
       </c>
       <c r="C70">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="D70">
-        <v>2240112</v>
+        <v>2238333</v>
       </c>
       <c r="E70" t="s">
         <v>13</v>
@@ -2457,10 +2457,10 @@
         <v>9</v>
       </c>
       <c r="C71">
-        <v>2145</v>
+        <v>2141</v>
       </c>
       <c r="D71">
-        <v>2681681</v>
+        <v>2679059</v>
       </c>
       <c r="E71" t="s">
         <v>13</v>
@@ -2483,10 +2483,10 @@
         <v>9</v>
       </c>
       <c r="C72">
-        <v>4158</v>
+        <v>4148</v>
       </c>
       <c r="D72">
-        <v>5565166</v>
+        <v>5554576</v>
       </c>
       <c r="E72" t="s">
         <v>13</v>
@@ -2509,10 +2509,10 @@
         <v>9</v>
       </c>
       <c r="C73">
-        <v>2052</v>
+        <v>2050</v>
       </c>
       <c r="D73">
-        <v>2490505</v>
+        <v>2490005</v>
       </c>
       <c r="E73" t="s">
         <v>13</v>
@@ -2535,10 +2535,10 @@
         <v>9</v>
       </c>
       <c r="C74">
-        <v>7809</v>
+        <v>7803</v>
       </c>
       <c r="D74">
-        <v>9783949</v>
+        <v>9781765</v>
       </c>
       <c r="E74" t="s">
         <v>13</v>
@@ -2561,10 +2561,10 @@
         <v>9</v>
       </c>
       <c r="C75">
-        <v>837</v>
+        <v>829</v>
       </c>
       <c r="D75">
-        <v>1159717</v>
+        <v>1147717</v>
       </c>
       <c r="E75" t="s">
         <v>14</v>
@@ -2587,10 +2587,10 @@
         <v>9</v>
       </c>
       <c r="C76">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="D76">
-        <v>987364</v>
+        <v>979864</v>
       </c>
       <c r="E76" t="s">
         <v>14</v>
@@ -2639,10 +2639,10 @@
         <v>9</v>
       </c>
       <c r="C78">
-        <v>1923</v>
+        <v>1914</v>
       </c>
       <c r="D78">
-        <v>2732909</v>
+        <v>2719409</v>
       </c>
       <c r="E78" t="s">
         <v>14</v>
@@ -2665,10 +2665,10 @@
         <v>9</v>
       </c>
       <c r="C79">
-        <v>1993</v>
+        <v>1967</v>
       </c>
       <c r="D79">
-        <v>2759795</v>
+        <v>2724566</v>
       </c>
       <c r="E79" t="s">
         <v>14</v>
@@ -2691,10 +2691,10 @@
         <v>9</v>
       </c>
       <c r="C80">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D80">
-        <v>389953</v>
+        <v>386953</v>
       </c>
       <c r="E80" t="s">
         <v>14</v>
@@ -2717,10 +2717,10 @@
         <v>9</v>
       </c>
       <c r="C81">
-        <v>1768</v>
+        <v>1752</v>
       </c>
       <c r="D81">
-        <v>2522574</v>
+        <v>2498574</v>
       </c>
       <c r="E81" t="s">
         <v>14</v>
@@ -2743,10 +2743,10 @@
         <v>9</v>
       </c>
       <c r="C82">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D82">
-        <v>183394</v>
+        <v>180394</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2795,10 +2795,10 @@
         <v>9</v>
       </c>
       <c r="C84">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="D84">
-        <v>545976</v>
+        <v>542976</v>
       </c>
       <c r="E84" t="s">
         <v>14</v>
@@ -2821,10 +2821,10 @@
         <v>9</v>
       </c>
       <c r="C85">
-        <v>1299</v>
+        <v>1283</v>
       </c>
       <c r="D85">
-        <v>1805252</v>
+        <v>1784454</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
@@ -2847,10 +2847,10 @@
         <v>9</v>
       </c>
       <c r="C86">
-        <v>774</v>
+        <v>757</v>
       </c>
       <c r="D86">
-        <v>982399</v>
+        <v>960413</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
@@ -2873,10 +2873,10 @@
         <v>9</v>
       </c>
       <c r="C87">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="D87">
-        <v>509303</v>
+        <v>508827</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -2899,10 +2899,10 @@
         <v>9</v>
       </c>
       <c r="C88">
-        <v>773</v>
+        <v>765</v>
       </c>
       <c r="D88">
-        <v>1031402</v>
+        <v>1022928</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -2925,10 +2925,10 @@
         <v>9</v>
       </c>
       <c r="C89">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D89">
-        <v>494236</v>
+        <v>485733</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
@@ -2951,10 +2951,10 @@
         <v>9</v>
       </c>
       <c r="C90">
-        <v>1376</v>
+        <v>1368</v>
       </c>
       <c r="D90">
-        <v>1636054</v>
+        <v>1625864</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
@@ -2977,10 +2977,10 @@
         <v>9</v>
       </c>
       <c r="C91">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="D91">
-        <v>2365615</v>
+        <v>2364838</v>
       </c>
       <c r="E91" t="s">
         <v>15</v>
@@ -3107,10 +3107,10 @@
         <v>9</v>
       </c>
       <c r="C96">
-        <v>12361</v>
+        <v>12359</v>
       </c>
       <c r="D96">
-        <v>17825886</v>
+        <v>17822886</v>
       </c>
       <c r="E96" t="s">
         <v>15</v>
@@ -3133,10 +3133,10 @@
         <v>9</v>
       </c>
       <c r="C97">
-        <v>18193</v>
+        <v>18187</v>
       </c>
       <c r="D97">
-        <v>24441685</v>
+        <v>24435489</v>
       </c>
       <c r="E97" t="s">
         <v>15</v>
@@ -3185,10 +3185,10 @@
         <v>9</v>
       </c>
       <c r="C99">
-        <v>11827</v>
+        <v>11823</v>
       </c>
       <c r="D99">
-        <v>17128699</v>
+        <v>17126117</v>
       </c>
       <c r="E99" t="s">
         <v>15</v>
@@ -3211,10 +3211,10 @@
         <v>9</v>
       </c>
       <c r="C100">
-        <v>1370</v>
+        <v>1366</v>
       </c>
       <c r="D100">
-        <v>1752107</v>
+        <v>1748697</v>
       </c>
       <c r="E100" t="s">
         <v>15</v>
@@ -3263,10 +3263,10 @@
         <v>9</v>
       </c>
       <c r="C102">
-        <v>2094</v>
+        <v>2086</v>
       </c>
       <c r="D102">
-        <v>2863168</v>
+        <v>2852543</v>
       </c>
       <c r="E102" t="s">
         <v>15</v>
@@ -3289,10 +3289,10 @@
         <v>9</v>
       </c>
       <c r="C103">
-        <v>7348</v>
+        <v>7340</v>
       </c>
       <c r="D103">
-        <v>9880621</v>
+        <v>9871544</v>
       </c>
       <c r="E103" t="s">
         <v>15</v>
@@ -3315,10 +3315,10 @@
         <v>9</v>
       </c>
       <c r="C104">
-        <v>3459</v>
+        <v>3455</v>
       </c>
       <c r="D104">
-        <v>4398676</v>
+        <v>4392676</v>
       </c>
       <c r="E104" t="s">
         <v>15</v>
@@ -3341,10 +3341,10 @@
         <v>9</v>
       </c>
       <c r="C105">
-        <v>4410</v>
+        <v>4402</v>
       </c>
       <c r="D105">
-        <v>5403308</v>
+        <v>5400487</v>
       </c>
       <c r="E105" t="s">
         <v>15</v>
@@ -3367,10 +3367,10 @@
         <v>9</v>
       </c>
       <c r="C106">
-        <v>9106</v>
+        <v>9088</v>
       </c>
       <c r="D106">
-        <v>12467269</v>
+        <v>12453133</v>
       </c>
       <c r="E106" t="s">
         <v>15</v>
@@ -3393,10 +3393,10 @@
         <v>9</v>
       </c>
       <c r="C107">
-        <v>3809</v>
+        <v>3803</v>
       </c>
       <c r="D107">
-        <v>4502101</v>
+        <v>4496919</v>
       </c>
       <c r="E107" t="s">
         <v>15</v>
@@ -3419,10 +3419,10 @@
         <v>9</v>
       </c>
       <c r="C108">
-        <v>17207</v>
+        <v>17191</v>
       </c>
       <c r="D108">
-        <v>20880511</v>
+        <v>20875478</v>
       </c>
       <c r="E108" t="s">
         <v>15</v>
@@ -4225,10 +4225,10 @@
         <v>9</v>
       </c>
       <c r="C139">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D139">
-        <v>220098</v>
+        <v>217858</v>
       </c>
       <c r="E139" t="s">
         <v>17</v>
@@ -4433,10 +4433,10 @@
         <v>9</v>
       </c>
       <c r="C147">
-        <v>10932</v>
+        <v>10924</v>
       </c>
       <c r="D147">
-        <v>15525510</v>
+        <v>15517990</v>
       </c>
       <c r="E147" t="s">
         <v>18</v>
@@ -4459,10 +4459,10 @@
         <v>9</v>
       </c>
       <c r="C148">
-        <v>18609</v>
+        <v>18601</v>
       </c>
       <c r="D148">
-        <v>23944512</v>
+        <v>23940912</v>
       </c>
       <c r="E148" t="s">
         <v>18</v>
@@ -4485,10 +4485,10 @@
         <v>9</v>
       </c>
       <c r="C149">
-        <v>3985</v>
+        <v>3973</v>
       </c>
       <c r="D149">
-        <v>5489807</v>
+        <v>5472972</v>
       </c>
       <c r="E149" t="s">
         <v>18</v>
@@ -4537,10 +4537,10 @@
         <v>9</v>
       </c>
       <c r="C151">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="D151">
-        <v>1698152</v>
+        <v>1695152</v>
       </c>
       <c r="E151" t="s">
         <v>18</v>
@@ -4589,10 +4589,10 @@
         <v>9</v>
       </c>
       <c r="C153">
-        <v>2125</v>
+        <v>2121</v>
       </c>
       <c r="D153">
-        <v>2869367</v>
+        <v>2863367</v>
       </c>
       <c r="E153" t="s">
         <v>18</v>
@@ -4615,10 +4615,10 @@
         <v>9</v>
       </c>
       <c r="C154">
-        <v>7553</v>
+        <v>7534</v>
       </c>
       <c r="D154">
-        <v>10244977</v>
+        <v>10225829</v>
       </c>
       <c r="E154" t="s">
         <v>18</v>
@@ -4641,10 +4641,10 @@
         <v>9</v>
       </c>
       <c r="C155">
-        <v>3602</v>
+        <v>3596</v>
       </c>
       <c r="D155">
-        <v>4520909</v>
+        <v>4516560</v>
       </c>
       <c r="E155" t="s">
         <v>18</v>
@@ -4667,10 +4667,10 @@
         <v>9</v>
       </c>
       <c r="C156">
-        <v>4025</v>
+        <v>4019</v>
       </c>
       <c r="D156">
-        <v>5035906</v>
+        <v>5029036</v>
       </c>
       <c r="E156" t="s">
         <v>18</v>
@@ -4693,10 +4693,10 @@
         <v>9</v>
       </c>
       <c r="C157">
-        <v>9451</v>
+        <v>9438</v>
       </c>
       <c r="D157">
-        <v>12903422</v>
+        <v>12892396</v>
       </c>
       <c r="E157" t="s">
         <v>18</v>
@@ -4719,10 +4719,10 @@
         <v>9</v>
       </c>
       <c r="C158">
-        <v>3831</v>
+        <v>3820</v>
       </c>
       <c r="D158">
-        <v>4594378</v>
+        <v>4588299</v>
       </c>
       <c r="E158" t="s">
         <v>18</v>
@@ -4745,10 +4745,10 @@
         <v>9</v>
       </c>
       <c r="C159">
-        <v>17279</v>
+        <v>17263</v>
       </c>
       <c r="D159">
-        <v>20419349</v>
+        <v>20409574</v>
       </c>
       <c r="E159" t="s">
         <v>18</v>
@@ -5005,10 +5005,10 @@
         <v>9</v>
       </c>
       <c r="C169">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D169">
-        <v>484581</v>
+        <v>483081</v>
       </c>
       <c r="E169" t="s">
         <v>19</v>
@@ -5083,10 +5083,10 @@
         <v>9</v>
       </c>
       <c r="C172">
-        <v>1706</v>
+        <v>1702</v>
       </c>
       <c r="D172">
-        <v>2414521</v>
+        <v>2409511</v>
       </c>
       <c r="E172" t="s">
         <v>19</v>
@@ -5135,10 +5135,10 @@
         <v>9</v>
       </c>
       <c r="C174">
-        <v>1493</v>
+        <v>1489</v>
       </c>
       <c r="D174">
-        <v>1941414</v>
+        <v>1936902</v>
       </c>
       <c r="E174" t="s">
         <v>19</v>
@@ -5161,10 +5161,10 @@
         <v>9</v>
       </c>
       <c r="C175">
-        <v>2124</v>
+        <v>2116</v>
       </c>
       <c r="D175">
-        <v>2998626</v>
+        <v>2986761</v>
       </c>
       <c r="E175" t="s">
         <v>19</v>
@@ -5187,10 +5187,10 @@
         <v>9</v>
       </c>
       <c r="C176">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="D176">
-        <v>1071026</v>
+        <v>1069676</v>
       </c>
       <c r="E176" t="s">
         <v>19</v>
@@ -5421,10 +5421,10 @@
         <v>9</v>
       </c>
       <c r="C185">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D185">
-        <v>201482</v>
+        <v>201382</v>
       </c>
       <c r="E185" t="s">
         <v>20</v>
@@ -5551,10 +5551,10 @@
         <v>9</v>
       </c>
       <c r="C190">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D190">
-        <v>597467</v>
+        <v>594467</v>
       </c>
       <c r="E190" t="s">
         <v>20</v>
@@ -5603,10 +5603,10 @@
         <v>9</v>
       </c>
       <c r="C192">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D192">
-        <v>380613</v>
+        <v>380415</v>
       </c>
       <c r="E192" t="s">
         <v>20</v>
@@ -5655,10 +5655,10 @@
         <v>9</v>
       </c>
       <c r="C194">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D194">
-        <v>123364</v>
+        <v>120364</v>
       </c>
       <c r="E194" t="s">
         <v>21</v>
@@ -5681,10 +5681,10 @@
         <v>9</v>
       </c>
       <c r="C195">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D195">
-        <v>116624</v>
+        <v>113624</v>
       </c>
       <c r="E195" t="s">
         <v>21</v>
@@ -5733,10 +5733,10 @@
         <v>9</v>
       </c>
       <c r="C197">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D197">
-        <v>300741</v>
+        <v>297741</v>
       </c>
       <c r="E197" t="s">
         <v>21</v>
@@ -5759,10 +5759,10 @@
         <v>9</v>
       </c>
       <c r="C198">
-        <v>521</v>
+        <v>514</v>
       </c>
       <c r="D198">
-        <v>725246</v>
+        <v>719636</v>
       </c>
       <c r="E198" t="s">
         <v>21</v>
@@ -5785,10 +5785,10 @@
         <v>9</v>
       </c>
       <c r="C199">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D199">
-        <v>207059</v>
+        <v>201059</v>
       </c>
       <c r="E199" t="s">
         <v>21</v>
@@ -5811,10 +5811,10 @@
         <v>9</v>
       </c>
       <c r="C200">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D200">
-        <v>224291</v>
+        <v>221291</v>
       </c>
       <c r="E200" t="s">
         <v>21</v>
@@ -6045,10 +6045,10 @@
         <v>9</v>
       </c>
       <c r="C209">
-        <v>1234</v>
+        <v>1232</v>
       </c>
       <c r="D209">
-        <v>1674206</v>
+        <v>1671206</v>
       </c>
       <c r="E209" t="s">
         <v>22</v>
@@ -6071,10 +6071,10 @@
         <v>9</v>
       </c>
       <c r="C210">
-        <v>2290</v>
+        <v>2288</v>
       </c>
       <c r="D210">
-        <v>2850846</v>
+        <v>2850512</v>
       </c>
       <c r="E210" t="s">
         <v>22</v>
@@ -6149,10 +6149,10 @@
         <v>9</v>
       </c>
       <c r="C213">
-        <v>6583</v>
+        <v>6581</v>
       </c>
       <c r="D213">
-        <v>9426699</v>
+        <v>9424699</v>
       </c>
       <c r="E213" t="s">
         <v>22</v>
@@ -6175,10 +6175,10 @@
         <v>9</v>
       </c>
       <c r="C214">
-        <v>12045</v>
+        <v>12035</v>
       </c>
       <c r="D214">
-        <v>15954722</v>
+        <v>15944464</v>
       </c>
       <c r="E214" t="s">
         <v>22</v>
@@ -6201,10 +6201,10 @@
         <v>9</v>
       </c>
       <c r="C215">
-        <v>1349</v>
+        <v>1347</v>
       </c>
       <c r="D215">
-        <v>1843939</v>
+        <v>1840939</v>
       </c>
       <c r="E215" t="s">
         <v>22</v>
@@ -6227,10 +6227,10 @@
         <v>9</v>
       </c>
       <c r="C216">
-        <v>7966</v>
+        <v>7958</v>
       </c>
       <c r="D216">
-        <v>11432171</v>
+        <v>11426908</v>
       </c>
       <c r="E216" t="s">
         <v>22</v>
@@ -6253,10 +6253,10 @@
         <v>9</v>
       </c>
       <c r="C217">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="D217">
-        <v>883568</v>
+        <v>880568</v>
       </c>
       <c r="E217" t="s">
         <v>22</v>
@@ -6331,10 +6331,10 @@
         <v>9</v>
       </c>
       <c r="C220">
-        <v>4315</v>
+        <v>4307</v>
       </c>
       <c r="D220">
-        <v>5847715</v>
+        <v>5835829</v>
       </c>
       <c r="E220" t="s">
         <v>22</v>
@@ -6357,10 +6357,10 @@
         <v>9</v>
       </c>
       <c r="C221">
-        <v>2037</v>
+        <v>2033</v>
       </c>
       <c r="D221">
-        <v>2535576</v>
+        <v>2533128</v>
       </c>
       <c r="E221" t="s">
         <v>22</v>
@@ -6383,10 +6383,10 @@
         <v>9</v>
       </c>
       <c r="C222">
-        <v>2586</v>
+        <v>2574</v>
       </c>
       <c r="D222">
-        <v>3111588</v>
+        <v>3105749</v>
       </c>
       <c r="E222" t="s">
         <v>22</v>
@@ -6409,10 +6409,10 @@
         <v>9</v>
       </c>
       <c r="C223">
-        <v>4973</v>
+        <v>4961</v>
       </c>
       <c r="D223">
-        <v>6660357</v>
+        <v>6644354</v>
       </c>
       <c r="E223" t="s">
         <v>22</v>
@@ -6435,10 +6435,10 @@
         <v>9</v>
       </c>
       <c r="C224">
-        <v>2508</v>
+        <v>2506</v>
       </c>
       <c r="D224">
-        <v>3044892</v>
+        <v>3042863</v>
       </c>
       <c r="E224" t="s">
         <v>22</v>
@@ -6461,10 +6461,10 @@
         <v>9</v>
       </c>
       <c r="C225">
-        <v>10533</v>
+        <v>10524</v>
       </c>
       <c r="D225">
-        <v>12967196</v>
+        <v>12960387</v>
       </c>
       <c r="E225" t="s">
         <v>22</v>
@@ -6539,10 +6539,10 @@
         <v>9</v>
       </c>
       <c r="C228">
-        <v>7192</v>
+        <v>7186</v>
       </c>
       <c r="D228">
-        <v>8793264</v>
+        <v>8784728</v>
       </c>
       <c r="E228" t="s">
         <v>23</v>
@@ -6617,10 +6617,10 @@
         <v>9</v>
       </c>
       <c r="C231">
-        <v>19321</v>
+        <v>19317</v>
       </c>
       <c r="D231">
-        <v>27515812</v>
+        <v>27509812</v>
       </c>
       <c r="E231" t="s">
         <v>23</v>
@@ -6643,10 +6643,10 @@
         <v>9</v>
       </c>
       <c r="C232">
-        <v>27715</v>
+        <v>27700</v>
       </c>
       <c r="D232">
-        <v>36828238</v>
+        <v>36816161</v>
       </c>
       <c r="E232" t="s">
         <v>23</v>
@@ -6669,10 +6669,10 @@
         <v>9</v>
       </c>
       <c r="C233">
-        <v>3563</v>
+        <v>3561</v>
       </c>
       <c r="D233">
-        <v>4863582</v>
+        <v>4860582</v>
       </c>
       <c r="E233" t="s">
         <v>23</v>
@@ -6695,10 +6695,10 @@
         <v>9</v>
       </c>
       <c r="C234">
-        <v>17879</v>
+        <v>17875</v>
       </c>
       <c r="D234">
-        <v>25312914</v>
+        <v>25306914</v>
       </c>
       <c r="E234" t="s">
         <v>23</v>
@@ -6721,10 +6721,10 @@
         <v>9</v>
       </c>
       <c r="C235">
-        <v>2181</v>
+        <v>2175</v>
       </c>
       <c r="D235">
-        <v>2816466</v>
+        <v>2810598</v>
       </c>
       <c r="E235" t="s">
         <v>23</v>
@@ -6773,10 +6773,10 @@
         <v>9</v>
       </c>
       <c r="C237">
-        <v>4339</v>
+        <v>4327</v>
       </c>
       <c r="D237">
-        <v>5809122</v>
+        <v>5795807</v>
       </c>
       <c r="E237" t="s">
         <v>23</v>
@@ -6799,10 +6799,10 @@
         <v>9</v>
       </c>
       <c r="C238">
-        <v>12865</v>
+        <v>12849</v>
       </c>
       <c r="D238">
-        <v>17280059</v>
+        <v>17268357</v>
       </c>
       <c r="E238" t="s">
         <v>23</v>
@@ -6825,10 +6825,10 @@
         <v>9</v>
       </c>
       <c r="C239">
-        <v>6689</v>
+        <v>6683</v>
       </c>
       <c r="D239">
-        <v>8338710</v>
+        <v>8333044</v>
       </c>
       <c r="E239" t="s">
         <v>23</v>
@@ -6851,10 +6851,10 @@
         <v>9</v>
       </c>
       <c r="C240">
-        <v>7450</v>
+        <v>7424</v>
       </c>
       <c r="D240">
-        <v>8768715</v>
+        <v>8744832</v>
       </c>
       <c r="E240" t="s">
         <v>23</v>
@@ -6877,10 +6877,10 @@
         <v>9</v>
       </c>
       <c r="C241">
-        <v>16275</v>
+        <v>16248</v>
       </c>
       <c r="D241">
-        <v>21638391</v>
+        <v>21614146</v>
       </c>
       <c r="E241" t="s">
         <v>23</v>
@@ -6903,10 +6903,10 @@
         <v>9</v>
       </c>
       <c r="C242">
-        <v>6270</v>
+        <v>6262</v>
       </c>
       <c r="D242">
-        <v>7544316</v>
+        <v>7538030</v>
       </c>
       <c r="E242" t="s">
         <v>23</v>
@@ -6929,10 +6929,10 @@
         <v>9</v>
       </c>
       <c r="C243">
-        <v>23268</v>
+        <v>23248</v>
       </c>
       <c r="D243">
-        <v>28402667</v>
+        <v>28392261</v>
       </c>
       <c r="E243" t="s">
         <v>23</v>
@@ -6955,10 +6955,10 @@
         <v>9</v>
       </c>
       <c r="C244">
-        <v>4341</v>
+        <v>4337</v>
       </c>
       <c r="D244">
-        <v>5850659</v>
+        <v>5845801</v>
       </c>
       <c r="E244" t="s">
         <v>24</v>
@@ -7007,10 +7007,10 @@
         <v>9</v>
       </c>
       <c r="C246">
-        <v>7346</v>
+        <v>7336</v>
       </c>
       <c r="D246">
-        <v>9023486</v>
+        <v>9014229</v>
       </c>
       <c r="E246" t="s">
         <v>24</v>
@@ -7085,10 +7085,10 @@
         <v>9</v>
       </c>
       <c r="C249">
-        <v>23482</v>
+        <v>23476</v>
       </c>
       <c r="D249">
-        <v>33286844</v>
+        <v>33277844</v>
       </c>
       <c r="E249" t="s">
         <v>24</v>
@@ -7111,10 +7111,10 @@
         <v>9</v>
       </c>
       <c r="C250">
-        <v>30120</v>
+        <v>30095</v>
       </c>
       <c r="D250">
-        <v>39659431</v>
+        <v>39631747</v>
       </c>
       <c r="E250" t="s">
         <v>24</v>
@@ -7137,10 +7137,10 @@
         <v>9</v>
       </c>
       <c r="C251">
-        <v>3812</v>
+        <v>3810</v>
       </c>
       <c r="D251">
-        <v>5077446</v>
+        <v>5076306</v>
       </c>
       <c r="E251" t="s">
         <v>24</v>
@@ -7163,10 +7163,10 @@
         <v>9</v>
       </c>
       <c r="C252">
-        <v>20494</v>
+        <v>20480</v>
       </c>
       <c r="D252">
-        <v>29025728</v>
+        <v>29009942</v>
       </c>
       <c r="E252" t="s">
         <v>24</v>
@@ -7215,10 +7215,10 @@
         <v>9</v>
       </c>
       <c r="C254">
-        <v>1200</v>
+        <v>1198</v>
       </c>
       <c r="D254">
-        <v>1663022</v>
+        <v>1661313</v>
       </c>
       <c r="E254" t="s">
         <v>24</v>
@@ -7241,10 +7241,10 @@
         <v>9</v>
       </c>
       <c r="C255">
-        <v>4951</v>
+        <v>4939</v>
       </c>
       <c r="D255">
-        <v>6654433</v>
+        <v>6640417</v>
       </c>
       <c r="E255" t="s">
         <v>24</v>
@@ -7267,10 +7267,10 @@
         <v>9</v>
       </c>
       <c r="C256">
-        <v>13977</v>
+        <v>13961</v>
       </c>
       <c r="D256">
-        <v>18978010</v>
+        <v>18961760</v>
       </c>
       <c r="E256" t="s">
         <v>24</v>
@@ -7293,10 +7293,10 @@
         <v>9</v>
       </c>
       <c r="C257">
-        <v>7076</v>
+        <v>7072</v>
       </c>
       <c r="D257">
-        <v>8819148</v>
+        <v>8817714</v>
       </c>
       <c r="E257" t="s">
         <v>24</v>
@@ -7345,10 +7345,10 @@
         <v>9</v>
       </c>
       <c r="C259">
-        <v>8849</v>
+        <v>8829</v>
       </c>
       <c r="D259">
-        <v>10402913</v>
+        <v>10389142</v>
       </c>
       <c r="E259" t="s">
         <v>24</v>
@@ -7371,10 +7371,10 @@
         <v>9</v>
       </c>
       <c r="C260">
-        <v>15906</v>
+        <v>15875</v>
       </c>
       <c r="D260">
-        <v>21106252</v>
+        <v>21074913</v>
       </c>
       <c r="E260" t="s">
         <v>24</v>
@@ -7397,10 +7397,10 @@
         <v>9</v>
       </c>
       <c r="C261">
-        <v>7090</v>
+        <v>7071</v>
       </c>
       <c r="D261">
-        <v>8473039</v>
+        <v>8453975</v>
       </c>
       <c r="E261" t="s">
         <v>24</v>
@@ -7423,10 +7423,10 @@
         <v>9</v>
       </c>
       <c r="C262">
-        <v>22940</v>
+        <v>22924</v>
       </c>
       <c r="D262">
-        <v>26910504</v>
+        <v>26899782</v>
       </c>
       <c r="E262" t="s">
         <v>24</v>
@@ -7449,10 +7449,10 @@
         <v>9</v>
       </c>
       <c r="C263">
-        <v>1563</v>
+        <v>1559</v>
       </c>
       <c r="D263">
-        <v>2161034</v>
+        <v>2157177</v>
       </c>
       <c r="E263" t="s">
         <v>25</v>
@@ -7501,10 +7501,10 @@
         <v>9</v>
       </c>
       <c r="C265">
-        <v>3098</v>
+        <v>3094</v>
       </c>
       <c r="D265">
-        <v>3810580</v>
+        <v>3807049</v>
       </c>
       <c r="E265" t="s">
         <v>25</v>
@@ -7579,10 +7579,10 @@
         <v>9</v>
       </c>
       <c r="C268">
-        <v>7656</v>
+        <v>7652</v>
       </c>
       <c r="D268">
-        <v>11000749</v>
+        <v>10994749</v>
       </c>
       <c r="E268" t="s">
         <v>25</v>
@@ -7605,10 +7605,10 @@
         <v>9</v>
       </c>
       <c r="C269">
-        <v>12587</v>
+        <v>12583</v>
       </c>
       <c r="D269">
-        <v>16676091</v>
+        <v>16670384</v>
       </c>
       <c r="E269" t="s">
         <v>25</v>
@@ -7631,10 +7631,10 @@
         <v>9</v>
       </c>
       <c r="C270">
-        <v>1592</v>
+        <v>1586</v>
       </c>
       <c r="D270">
-        <v>2224145</v>
+        <v>2215996</v>
       </c>
       <c r="E270" t="s">
         <v>25</v>
@@ -7735,10 +7735,10 @@
         <v>9</v>
       </c>
       <c r="C274">
-        <v>2246</v>
+        <v>2242</v>
       </c>
       <c r="D274">
-        <v>3037708</v>
+        <v>3032173</v>
       </c>
       <c r="E274" t="s">
         <v>25</v>
@@ -7761,10 +7761,10 @@
         <v>9</v>
       </c>
       <c r="C275">
-        <v>6603</v>
+        <v>6585</v>
       </c>
       <c r="D275">
-        <v>8949064</v>
+        <v>8932196</v>
       </c>
       <c r="E275" t="s">
         <v>25</v>
@@ -7787,10 +7787,10 @@
         <v>9</v>
       </c>
       <c r="C276">
-        <v>2554</v>
+        <v>2550</v>
       </c>
       <c r="D276">
-        <v>3285372</v>
+        <v>3281892</v>
       </c>
       <c r="E276" t="s">
         <v>25</v>
@@ -7813,10 +7813,10 @@
         <v>9</v>
       </c>
       <c r="C277">
-        <v>3229</v>
+        <v>3227</v>
       </c>
       <c r="D277">
-        <v>3942839</v>
+        <v>3940149</v>
       </c>
       <c r="E277" t="s">
         <v>25</v>
@@ -7839,10 +7839,10 @@
         <v>9</v>
       </c>
       <c r="C278">
-        <v>9078</v>
+        <v>9060</v>
       </c>
       <c r="D278">
-        <v>12159296</v>
+        <v>12141113</v>
       </c>
       <c r="E278" t="s">
         <v>25</v>
@@ -7865,10 +7865,10 @@
         <v>9</v>
       </c>
       <c r="C279">
-        <v>3411</v>
+        <v>3403</v>
       </c>
       <c r="D279">
-        <v>4130551</v>
+        <v>4123099</v>
       </c>
       <c r="E279" t="s">
         <v>25</v>
@@ -7891,10 +7891,10 @@
         <v>9</v>
       </c>
       <c r="C280">
-        <v>12130</v>
+        <v>12120</v>
       </c>
       <c r="D280">
-        <v>15196918</v>
+        <v>15193865</v>
       </c>
       <c r="E280" t="s">
         <v>25</v>
@@ -7969,10 +7969,10 @@
         <v>9</v>
       </c>
       <c r="C283">
-        <v>7224</v>
+        <v>7218</v>
       </c>
       <c r="D283">
-        <v>9330849</v>
+        <v>9322614</v>
       </c>
       <c r="E283" t="s">
         <v>26</v>
@@ -8047,10 +8047,10 @@
         <v>9</v>
       </c>
       <c r="C286">
-        <v>20559</v>
+        <v>20555</v>
       </c>
       <c r="D286">
-        <v>29351093</v>
+        <v>29345093</v>
       </c>
       <c r="E286" t="s">
         <v>26</v>
@@ -8073,10 +8073,10 @@
         <v>9</v>
       </c>
       <c r="C287">
-        <v>32379</v>
+        <v>32370</v>
       </c>
       <c r="D287">
-        <v>43287123</v>
+        <v>43276527</v>
       </c>
       <c r="E287" t="s">
         <v>26</v>
@@ -8099,10 +8099,10 @@
         <v>9</v>
       </c>
       <c r="C288">
-        <v>7054</v>
+        <v>7048</v>
       </c>
       <c r="D288">
-        <v>9851000</v>
+        <v>9847562</v>
       </c>
       <c r="E288" t="s">
         <v>26</v>
@@ -8125,10 +8125,10 @@
         <v>9</v>
       </c>
       <c r="C289">
-        <v>20072</v>
+        <v>20066</v>
       </c>
       <c r="D289">
-        <v>28952255</v>
+        <v>28944511</v>
       </c>
       <c r="E289" t="s">
         <v>26</v>
@@ -8151,10 +8151,10 @@
         <v>9</v>
       </c>
       <c r="C290">
-        <v>2834</v>
+        <v>2828</v>
       </c>
       <c r="D290">
-        <v>3698294</v>
+        <v>3689294</v>
       </c>
       <c r="E290" t="s">
         <v>26</v>
@@ -8177,10 +8177,10 @@
         <v>9</v>
       </c>
       <c r="C291">
-        <v>1371</v>
+        <v>1369</v>
       </c>
       <c r="D291">
-        <v>1942754</v>
+        <v>1940154</v>
       </c>
       <c r="E291" t="s">
         <v>26</v>
@@ -8203,10 +8203,10 @@
         <v>9</v>
       </c>
       <c r="C292">
-        <v>6012</v>
+        <v>5998</v>
       </c>
       <c r="D292">
-        <v>8346765</v>
+        <v>8329969</v>
       </c>
       <c r="E292" t="s">
         <v>26</v>
@@ -8229,10 +8229,10 @@
         <v>9</v>
       </c>
       <c r="C293">
-        <v>15672</v>
+        <v>15644</v>
       </c>
       <c r="D293">
-        <v>21377698</v>
+        <v>21346693</v>
       </c>
       <c r="E293" t="s">
         <v>26</v>
@@ -8255,10 +8255,10 @@
         <v>9</v>
       </c>
       <c r="C294">
-        <v>8675</v>
+        <v>8673</v>
       </c>
       <c r="D294">
-        <v>11177283</v>
+        <v>11174283</v>
       </c>
       <c r="E294" t="s">
         <v>26</v>
@@ -8307,10 +8307,10 @@
         <v>9</v>
       </c>
       <c r="C296">
-        <v>9799</v>
+        <v>9783</v>
       </c>
       <c r="D296">
-        <v>12025676</v>
+        <v>12013333</v>
       </c>
       <c r="E296" t="s">
         <v>26</v>
@@ -8333,10 +8333,10 @@
         <v>9</v>
       </c>
       <c r="C297">
-        <v>15550</v>
+        <v>15522</v>
       </c>
       <c r="D297">
-        <v>20715768</v>
+        <v>20689690</v>
       </c>
       <c r="E297" t="s">
         <v>26</v>
@@ -8359,10 +8359,10 @@
         <v>9</v>
       </c>
       <c r="C298">
-        <v>6937</v>
+        <v>6913</v>
       </c>
       <c r="D298">
-        <v>8604539</v>
+        <v>8584182</v>
       </c>
       <c r="E298" t="s">
         <v>26</v>
@@ -8385,10 +8385,10 @@
         <v>9</v>
       </c>
       <c r="C299">
-        <v>22257</v>
+        <v>22241</v>
       </c>
       <c r="D299">
-        <v>26782599</v>
+        <v>26764792</v>
       </c>
       <c r="E299" t="s">
         <v>26</v>
@@ -8437,10 +8437,10 @@
         <v>9</v>
       </c>
       <c r="C301">
-        <v>8195</v>
+        <v>8193</v>
       </c>
       <c r="D301">
-        <v>10957923</v>
+        <v>10955833</v>
       </c>
       <c r="E301" t="s">
         <v>27</v>
@@ -8515,10 +8515,10 @@
         <v>9</v>
       </c>
       <c r="C304">
-        <v>23935</v>
+        <v>23917</v>
       </c>
       <c r="D304">
-        <v>34581718</v>
+        <v>34559723</v>
       </c>
       <c r="E304" t="s">
         <v>27</v>
@@ -8541,10 +8541,10 @@
         <v>9</v>
       </c>
       <c r="C305">
-        <v>44310</v>
+        <v>44293</v>
       </c>
       <c r="D305">
-        <v>60918743</v>
+        <v>60897781</v>
       </c>
       <c r="E305" t="s">
         <v>27</v>
@@ -8567,10 +8567,10 @@
         <v>9</v>
       </c>
       <c r="C306">
-        <v>47038</v>
+        <v>47004</v>
       </c>
       <c r="D306">
-        <v>67823001</v>
+        <v>67784119</v>
       </c>
       <c r="E306" t="s">
         <v>27</v>
@@ -8593,10 +8593,10 @@
         <v>9</v>
       </c>
       <c r="C307">
-        <v>27002</v>
+        <v>26990</v>
       </c>
       <c r="D307">
-        <v>39763714</v>
+        <v>39749347</v>
       </c>
       <c r="E307" t="s">
         <v>27</v>
@@ -8619,10 +8619,10 @@
         <v>9</v>
       </c>
       <c r="C308">
-        <v>11979</v>
+        <v>11948</v>
       </c>
       <c r="D308">
-        <v>16433685</v>
+        <v>16394310</v>
       </c>
       <c r="E308" t="s">
         <v>27</v>
@@ -8645,10 +8645,10 @@
         <v>9</v>
       </c>
       <c r="C309">
-        <v>3019</v>
+        <v>3015</v>
       </c>
       <c r="D309">
-        <v>4330726</v>
+        <v>4324726</v>
       </c>
       <c r="E309" t="s">
         <v>27</v>
@@ -8671,10 +8671,10 @@
         <v>9</v>
       </c>
       <c r="C310">
-        <v>7882</v>
+        <v>7870</v>
       </c>
       <c r="D310">
-        <v>11229914</v>
+        <v>11212924</v>
       </c>
       <c r="E310" t="s">
         <v>27</v>
@@ -8697,10 +8697,10 @@
         <v>9</v>
       </c>
       <c r="C311">
-        <v>47833</v>
+        <v>47688</v>
       </c>
       <c r="D311">
-        <v>66171907</v>
+        <v>66004205</v>
       </c>
       <c r="E311" t="s">
         <v>27</v>
@@ -8723,10 +8723,10 @@
         <v>9</v>
       </c>
       <c r="C312">
-        <v>12699</v>
+        <v>12668</v>
       </c>
       <c r="D312">
-        <v>17022623</v>
+        <v>16991049</v>
       </c>
       <c r="E312" t="s">
         <v>27</v>
@@ -8775,10 +8775,10 @@
         <v>9</v>
       </c>
       <c r="C314">
-        <v>14009</v>
+        <v>13955</v>
       </c>
       <c r="D314">
-        <v>17436094</v>
+        <v>17383460</v>
       </c>
       <c r="E314" t="s">
         <v>27</v>
@@ -8801,10 +8801,10 @@
         <v>9</v>
       </c>
       <c r="C315">
-        <v>27111</v>
+        <v>27063</v>
       </c>
       <c r="D315">
-        <v>37047157</v>
+        <v>36996056</v>
       </c>
       <c r="E315" t="s">
         <v>27</v>
@@ -8827,10 +8827,10 @@
         <v>9</v>
       </c>
       <c r="C316">
-        <v>18258</v>
+        <v>18207</v>
       </c>
       <c r="D316">
-        <v>23602596</v>
+        <v>23553106</v>
       </c>
       <c r="E316" t="s">
         <v>27</v>
@@ -8853,10 +8853,10 @@
         <v>9</v>
       </c>
       <c r="C317">
-        <v>29116</v>
+        <v>29082</v>
       </c>
       <c r="D317">
-        <v>37972854</v>
+        <v>37942949</v>
       </c>
       <c r="E317" t="s">
         <v>27</v>

</xml_diff>